<commit_message>
Atualização de bases das ligas, do dia: 2024-01-31 às 21-30
</commit_message>
<xml_diff>
--- a/Croatia HNL/Croatia HNL.xlsx
+++ b/Croatia HNL/Croatia HNL.xlsx
@@ -9949,7 +9949,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>2808751</v>
+        <v>2798917</v>
       </c>
       <c r="C107" t="s">
         <v>28</v>
@@ -9961,13 +9961,13 @@
         <v>44338.5</v>
       </c>
       <c r="F107" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G107" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -9976,43 +9976,43 @@
         <v>43</v>
       </c>
       <c r="K107">
-        <v>1.4</v>
+        <v>2.75</v>
       </c>
       <c r="L107">
-        <v>4.333</v>
+        <v>3.4</v>
       </c>
       <c r="M107">
-        <v>6</v>
+        <v>2.2</v>
       </c>
       <c r="N107">
-        <v>1.4</v>
+        <v>4</v>
       </c>
       <c r="O107">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="P107">
-        <v>7.5</v>
+        <v>1.85</v>
       </c>
       <c r="Q107">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R107">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S107">
-        <v>1.75</v>
+        <v>1.9</v>
       </c>
       <c r="T107">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U107">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V107">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W107">
-        <v>0.3999999999999999</v>
+        <v>3</v>
       </c>
       <c r="X107">
         <v>-1</v>
@@ -10021,7 +10021,7 @@
         <v>-1</v>
       </c>
       <c r="Z107">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="AA107">
         <v>-1</v>
@@ -10030,7 +10030,7 @@
         <v>-1</v>
       </c>
       <c r="AC107">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="108" spans="1:29">
@@ -10038,7 +10038,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>2808752</v>
+        <v>2808751</v>
       </c>
       <c r="C108" t="s">
         <v>28</v>
@@ -10050,58 +10050,58 @@
         <v>44338.5</v>
       </c>
       <c r="F108" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G108" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H108">
         <v>2</v>
       </c>
       <c r="I108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J108" t="s">
         <v>43</v>
       </c>
       <c r="K108">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="L108">
-        <v>3.75</v>
+        <v>4.333</v>
       </c>
       <c r="M108">
-        <v>2.7</v>
+        <v>6</v>
       </c>
       <c r="N108">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="O108">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="P108">
-        <v>1.95</v>
+        <v>7.5</v>
       </c>
       <c r="Q108">
-        <v>0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R108">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="S108">
-        <v>1.9</v>
+        <v>1.75</v>
       </c>
       <c r="T108">
         <v>2.5</v>
       </c>
       <c r="U108">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V108">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W108">
-        <v>2.4</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="X108">
         <v>-1</v>
@@ -10110,16 +10110,16 @@
         <v>-1</v>
       </c>
       <c r="Z108">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
       <c r="AA108">
         <v>-1</v>
       </c>
       <c r="AB108">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC108">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="109" spans="1:29">
@@ -10127,7 +10127,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>2798917</v>
+        <v>2808752</v>
       </c>
       <c r="C109" t="s">
         <v>28</v>
@@ -10139,40 +10139,40 @@
         <v>44338.5</v>
       </c>
       <c r="F109" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G109" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H109">
+        <v>2</v>
+      </c>
+      <c r="I109">
         <v>1</v>
-      </c>
-      <c r="I109">
-        <v>0</v>
       </c>
       <c r="J109" t="s">
         <v>43</v>
       </c>
       <c r="K109">
-        <v>2.75</v>
+        <v>2.1</v>
       </c>
       <c r="L109">
+        <v>3.75</v>
+      </c>
+      <c r="M109">
+        <v>2.7</v>
+      </c>
+      <c r="N109">
         <v>3.4</v>
-      </c>
-      <c r="M109">
-        <v>2.2</v>
-      </c>
-      <c r="N109">
-        <v>4</v>
       </c>
       <c r="O109">
         <v>3.5</v>
       </c>
       <c r="P109">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="Q109">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R109">
         <v>1.95</v>
@@ -10181,16 +10181,16 @@
         <v>1.9</v>
       </c>
       <c r="T109">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U109">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V109">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W109">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="X109">
         <v>-1</v>
@@ -10205,10 +10205,10 @@
         <v>-1</v>
       </c>
       <c r="AB109">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC109">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="110" spans="1:29">
@@ -51491,10 +51491,10 @@
         <v>-1.5</v>
       </c>
       <c r="R574">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="S574">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="T574">
         <v>2.5</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-01 às 21-50
</commit_message>
<xml_diff>
--- a/Croatia HNL/Croatia HNL.xlsx
+++ b/Croatia HNL/Croatia HNL.xlsx
@@ -9949,7 +9949,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>2798917</v>
+        <v>2813294</v>
       </c>
       <c r="C107" t="s">
         <v>28</v>
@@ -9961,58 +9961,58 @@
         <v>44338.5</v>
       </c>
       <c r="F107" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G107" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H107">
+        <v>2</v>
+      </c>
+      <c r="I107">
         <v>1</v>
-      </c>
-      <c r="I107">
-        <v>0</v>
       </c>
       <c r="J107" t="s">
         <v>43</v>
       </c>
       <c r="K107">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="L107">
+        <v>3.2</v>
+      </c>
+      <c r="M107">
+        <v>3.3</v>
+      </c>
+      <c r="N107">
+        <v>1.8</v>
+      </c>
+      <c r="O107">
         <v>3.4</v>
       </c>
-      <c r="M107">
-        <v>2.2</v>
-      </c>
-      <c r="N107">
-        <v>4</v>
-      </c>
-      <c r="O107">
-        <v>3.5</v>
-      </c>
       <c r="P107">
+        <v>5</v>
+      </c>
+      <c r="Q107">
+        <v>-0.5</v>
+      </c>
+      <c r="R107">
         <v>1.85</v>
       </c>
-      <c r="Q107">
-        <v>0.5</v>
-      </c>
-      <c r="R107">
-        <v>1.95</v>
-      </c>
       <c r="S107">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="T107">
         <v>2.75</v>
       </c>
       <c r="U107">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V107">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W107">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="X107">
         <v>-1</v>
@@ -10021,16 +10021,16 @@
         <v>-1</v>
       </c>
       <c r="Z107">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA107">
         <v>-1</v>
       </c>
       <c r="AB107">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AC107">
-        <v>0.8500000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="108" spans="1:29">
@@ -10127,7 +10127,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>2808752</v>
+        <v>2798917</v>
       </c>
       <c r="C109" t="s">
         <v>28</v>
@@ -10139,40 +10139,40 @@
         <v>44338.5</v>
       </c>
       <c r="F109" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G109" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J109" t="s">
         <v>43</v>
       </c>
       <c r="K109">
-        <v>2.1</v>
+        <v>2.75</v>
       </c>
       <c r="L109">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="M109">
-        <v>2.7</v>
+        <v>2.2</v>
       </c>
       <c r="N109">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="O109">
         <v>3.5</v>
       </c>
       <c r="P109">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="Q109">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R109">
         <v>1.95</v>
@@ -10181,16 +10181,16 @@
         <v>1.9</v>
       </c>
       <c r="T109">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U109">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V109">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W109">
-        <v>2.4</v>
+        <v>3</v>
       </c>
       <c r="X109">
         <v>-1</v>
@@ -10205,10 +10205,10 @@
         <v>-1</v>
       </c>
       <c r="AB109">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC109">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="110" spans="1:29">
@@ -10216,7 +10216,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>2813294</v>
+        <v>2808752</v>
       </c>
       <c r="C110" t="s">
         <v>28</v>
@@ -10228,10 +10228,10 @@
         <v>44338.5</v>
       </c>
       <c r="F110" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G110" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H110">
         <v>2</v>
@@ -10243,43 +10243,43 @@
         <v>43</v>
       </c>
       <c r="K110">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="L110">
-        <v>3.2</v>
+        <v>3.75</v>
       </c>
       <c r="M110">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="N110">
-        <v>1.8</v>
+        <v>3.4</v>
       </c>
       <c r="O110">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P110">
-        <v>5</v>
+        <v>1.95</v>
       </c>
       <c r="Q110">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R110">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="S110">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="T110">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U110">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V110">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W110">
-        <v>0.8</v>
+        <v>2.4</v>
       </c>
       <c r="X110">
         <v>-1</v>
@@ -10288,16 +10288,16 @@
         <v>-1</v>
       </c>
       <c r="Z110">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AA110">
         <v>-1</v>
       </c>
       <c r="AB110">
-        <v>0.425</v>
+        <v>0.925</v>
       </c>
       <c r="AC110">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="111" spans="1:29">
@@ -51195,19 +51195,19 @@
         <v>-0.5</v>
       </c>
       <c r="R570">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S570">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T570">
         <v>2.5</v>
       </c>
       <c r="U570">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V570">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W570">
         <v>0</v>
@@ -51257,31 +51257,31 @@
         <v>5.75</v>
       </c>
       <c r="N571">
-        <v>1.6</v>
+        <v>1.65</v>
       </c>
       <c r="O571">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P571">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c r="Q571">
         <v>-0.75</v>
       </c>
       <c r="R571">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="S571">
-        <v>2.1</v>
+        <v>1.975</v>
       </c>
       <c r="T571">
         <v>2.5</v>
       </c>
       <c r="U571">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V571">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="W571">
         <v>0</v>
@@ -51331,31 +51331,31 @@
         <v>2.15</v>
       </c>
       <c r="N572">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="O572">
         <v>3.5</v>
       </c>
       <c r="P572">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="Q572">
         <v>0.25</v>
       </c>
       <c r="R572">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="S572">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="T572">
         <v>2.25</v>
       </c>
       <c r="U572">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V572">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W572">
         <v>0</v>
@@ -51405,22 +51405,22 @@
         <v>8.5</v>
       </c>
       <c r="N573">
-        <v>1.3</v>
+        <v>1.333</v>
       </c>
       <c r="O573">
         <v>6</v>
       </c>
       <c r="P573">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="Q573">
         <v>-1.5</v>
       </c>
       <c r="R573">
+        <v>1.95</v>
+      </c>
+      <c r="S573">
         <v>1.9</v>
-      </c>
-      <c r="S573">
-        <v>1.95</v>
       </c>
       <c r="T573">
         <v>3</v>
@@ -51479,31 +51479,31 @@
         <v>11</v>
       </c>
       <c r="N574">
-        <v>1.285</v>
+        <v>1.25</v>
       </c>
       <c r="O574">
         <v>5.75</v>
       </c>
       <c r="P574">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q574">
-        <v>-1.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R574">
+        <v>2</v>
+      </c>
+      <c r="S574">
+        <v>1.85</v>
+      </c>
+      <c r="T574">
+        <v>2.75</v>
+      </c>
+      <c r="U574">
+        <v>2.025</v>
+      </c>
+      <c r="V574">
         <v>1.825</v>
-      </c>
-      <c r="S574">
-        <v>2.025</v>
-      </c>
-      <c r="T574">
-        <v>2.5</v>
-      </c>
-      <c r="U574">
-        <v>1.825</v>
-      </c>
-      <c r="V574">
-        <v>2.025</v>
       </c>
       <c r="W574">
         <v>0</v>

</xml_diff>